<commit_message>
finish analyzing ki67 manualvsAperio
</commit_message>
<xml_diff>
--- a/KI67/data/aperio/TIAN TMA5 APERIO.xlsx
+++ b/KI67/data/aperio/TIAN TMA5 APERIO.xlsx
@@ -1,22 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26915"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markwang/github/LearnR/KI67/data/aperio/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-345" yWindow="-180" windowWidth="20325" windowHeight="8310"/>
+    <workbookView xWindow="20" yWindow="760" windowWidth="25600" windowHeight="14080" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="to txt" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'to txt'!$A$1:$B$16384</definedName>
+  </definedNames>
+  <calcPr calcId="150001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>CASE</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -45,6 +61,15 @@
     <t>TL</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>Percent</t>
+  </si>
+  <si>
+    <t>case</t>
+  </si>
+  <si>
+    <t>score</t>
+  </si>
 </sst>
 </file>
 
@@ -54,14 +79,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -70,7 +95,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -161,9 +186,26 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -174,7 +216,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -216,12 +258,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -251,12 +293,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -462,13 +504,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BL20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="BL19" sqref="BL1:BL19"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:64" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:64" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -656,7 +698,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="2" spans="1:64" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -836,7 +878,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:64" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:64" x14ac:dyDescent="0.2">
       <c r="B3" s="9">
         <v>6</v>
       </c>
@@ -1013,7 +1055,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:64" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:64" x14ac:dyDescent="0.2">
       <c r="B4" s="9">
         <v>38</v>
       </c>
@@ -1188,7 +1230,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:64" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:64" x14ac:dyDescent="0.2">
       <c r="B5" s="9">
         <v>9</v>
       </c>
@@ -1357,7 +1399,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:64" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:64" x14ac:dyDescent="0.2">
       <c r="B6" s="9">
         <v>9</v>
       </c>
@@ -1522,7 +1564,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:64" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:64" x14ac:dyDescent="0.2">
       <c r="B7" s="9">
         <v>45</v>
       </c>
@@ -1681,7 +1723,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:64" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:64" x14ac:dyDescent="0.2">
       <c r="B8" s="9">
         <v>10</v>
       </c>
@@ -1840,7 +1882,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:64" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:64" x14ac:dyDescent="0.2">
       <c r="B9" s="9">
         <v>7</v>
       </c>
@@ -1985,7 +2027,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:64" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:64" x14ac:dyDescent="0.2">
       <c r="B10" s="9">
         <v>28</v>
       </c>
@@ -2116,7 +2158,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:64" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:64" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>2</v>
       </c>
@@ -2364,7 +2406,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="12" spans="1:64" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:64" x14ac:dyDescent="0.2">
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
@@ -2429,7 +2471,7 @@
       <c r="BK12" s="2"/>
       <c r="BL12" s="6"/>
     </row>
-    <row r="13" spans="1:64" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:64" x14ac:dyDescent="0.2">
       <c r="B13" s="9">
         <v>373</v>
       </c>
@@ -2606,7 +2648,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="14" spans="1:64" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:64" x14ac:dyDescent="0.2">
       <c r="B14" s="9">
         <v>379</v>
       </c>
@@ -2781,7 +2823,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="15" spans="1:64" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:64" x14ac:dyDescent="0.2">
       <c r="B15" s="9">
         <v>506</v>
       </c>
@@ -2958,7 +3000,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="16" spans="1:64" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>3</v>
       </c>
@@ -3146,7 +3188,7 @@
       </c>
       <c r="AW16" s="5"/>
       <c r="AX16" s="7">
-        <f t="shared" ref="AW16:BL16" si="32">SUM(AX13:AX15)</f>
+        <f t="shared" ref="AX16:BL16" si="32">SUM(AX13:AX15)</f>
         <v>1109</v>
       </c>
       <c r="AY16" s="3">
@@ -3206,7 +3248,7 @@
         <v>1637</v>
       </c>
     </row>
-    <row r="17" spans="1:64" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:64" x14ac:dyDescent="0.2">
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
@@ -3271,7 +3313,7 @@
       <c r="BK17" s="2"/>
       <c r="BL17" s="6"/>
     </row>
-    <row r="18" spans="1:64" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:64" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>4</v>
       </c>
@@ -3459,7 +3501,7 @@
       </c>
       <c r="AW18" s="5"/>
       <c r="AX18" s="7">
-        <f t="shared" ref="AW18:BL18" si="34">(AX11/AX16)*100</f>
+        <f t="shared" ref="AX18:BL18" si="34">(AX11/AX16)*100</f>
         <v>9.9188458070333638</v>
       </c>
       <c r="AY18" s="3">
@@ -3519,7 +3561,7 @@
         <v>18.387293830177153</v>
       </c>
     </row>
-    <row r="19" spans="1:64" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:64" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>5</v>
       </c>
@@ -3700,7 +3742,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:64" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:64" x14ac:dyDescent="0.2">
       <c r="R20" s="4"/>
     </row>
   </sheetData>
@@ -3712,12 +3754,388 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:BL2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:64" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9">
+        <v>65</v>
+      </c>
+      <c r="C1" s="9">
+        <v>92</v>
+      </c>
+      <c r="D1" s="9">
+        <v>122</v>
+      </c>
+      <c r="E1" s="2">
+        <v>189</v>
+      </c>
+      <c r="F1" s="2">
+        <v>206</v>
+      </c>
+      <c r="G1" s="9">
+        <v>228</v>
+      </c>
+      <c r="H1" s="6">
+        <v>271</v>
+      </c>
+      <c r="I1" s="9">
+        <v>282</v>
+      </c>
+      <c r="J1" s="6">
+        <v>342</v>
+      </c>
+      <c r="K1" s="6">
+        <v>465</v>
+      </c>
+      <c r="L1" s="9">
+        <v>481</v>
+      </c>
+      <c r="M1" s="2">
+        <v>520</v>
+      </c>
+      <c r="N1" s="9">
+        <v>572</v>
+      </c>
+      <c r="O1" s="9">
+        <v>240</v>
+      </c>
+      <c r="P1" s="9">
+        <v>608</v>
+      </c>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="9">
+        <v>26</v>
+      </c>
+      <c r="S1" s="6">
+        <v>36</v>
+      </c>
+      <c r="T1" s="6">
+        <v>70</v>
+      </c>
+      <c r="U1" s="6">
+        <v>97</v>
+      </c>
+      <c r="V1" s="6">
+        <v>190</v>
+      </c>
+      <c r="W1" s="6">
+        <v>244</v>
+      </c>
+      <c r="X1" s="9">
+        <v>249</v>
+      </c>
+      <c r="Y1" s="9">
+        <v>295</v>
+      </c>
+      <c r="Z1" s="9">
+        <v>301</v>
+      </c>
+      <c r="AA1" s="9">
+        <v>353</v>
+      </c>
+      <c r="AB1" s="9">
+        <v>395</v>
+      </c>
+      <c r="AC1" s="6">
+        <v>413</v>
+      </c>
+      <c r="AD1" s="9">
+        <v>529</v>
+      </c>
+      <c r="AE1" s="2">
+        <v>641</v>
+      </c>
+      <c r="AF1" s="6">
+        <v>587</v>
+      </c>
+      <c r="AG1" s="4"/>
+      <c r="AH1" s="6">
+        <v>52</v>
+      </c>
+      <c r="AI1" s="9">
+        <v>89</v>
+      </c>
+      <c r="AJ1" s="6">
+        <v>98</v>
+      </c>
+      <c r="AK1" s="6">
+        <v>168</v>
+      </c>
+      <c r="AL1" s="9">
+        <v>341</v>
+      </c>
+      <c r="AM1" s="6">
+        <v>382</v>
+      </c>
+      <c r="AN1" s="9">
+        <v>408</v>
+      </c>
+      <c r="AO1" s="6">
+        <v>470</v>
+      </c>
+      <c r="AP1" s="9">
+        <v>487</v>
+      </c>
+      <c r="AQ1" s="9">
+        <v>513</v>
+      </c>
+      <c r="AR1" s="6">
+        <v>533</v>
+      </c>
+      <c r="AS1" s="9">
+        <v>616</v>
+      </c>
+      <c r="AT1" s="6">
+        <v>617</v>
+      </c>
+      <c r="AU1" s="9">
+        <v>620</v>
+      </c>
+      <c r="AV1" s="9">
+        <v>656</v>
+      </c>
+      <c r="AW1" s="4"/>
+      <c r="AX1" s="6">
+        <v>28</v>
+      </c>
+      <c r="AY1" s="2">
+        <v>414</v>
+      </c>
+      <c r="AZ1" s="6">
+        <v>472</v>
+      </c>
+      <c r="BA1" s="6">
+        <v>603</v>
+      </c>
+      <c r="BB1" s="6">
+        <v>634</v>
+      </c>
+      <c r="BC1" s="6">
+        <v>148</v>
+      </c>
+      <c r="BD1" s="2">
+        <v>364</v>
+      </c>
+      <c r="BE1" s="2">
+        <v>500</v>
+      </c>
+      <c r="BF1" s="6">
+        <v>126</v>
+      </c>
+      <c r="BG1" s="6">
+        <v>241</v>
+      </c>
+      <c r="BH1" s="2">
+        <v>321</v>
+      </c>
+      <c r="BI1" s="11">
+        <v>346</v>
+      </c>
+      <c r="BJ1" s="11">
+        <v>347</v>
+      </c>
+      <c r="BK1" s="2">
+        <v>426</v>
+      </c>
+      <c r="BL1" s="6">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="2" spans="1:64" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>13.116057233704293</v>
+      </c>
+      <c r="C2">
+        <v>10.632610632610632</v>
+      </c>
+      <c r="D2">
+        <v>8.615384615384615</v>
+      </c>
+      <c r="E2">
+        <v>14.437760296159185</v>
+      </c>
+      <c r="F2">
+        <v>27.860696517412936</v>
+      </c>
+      <c r="G2">
+        <v>5.1921079958463139</v>
+      </c>
+      <c r="H2">
+        <v>7.9720279720279716</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>35.61463543037641</v>
+      </c>
+      <c r="K2">
+        <v>13.043478260869565</v>
+      </c>
+      <c r="L2">
+        <v>12.558548009367682</v>
+      </c>
+      <c r="M2">
+        <v>6.2124248496993983</v>
+      </c>
+      <c r="N2">
+        <v>4</v>
+      </c>
+      <c r="O2">
+        <v>47.955145118733512</v>
+      </c>
+      <c r="P2">
+        <v>18.52367688022284</v>
+      </c>
+      <c r="R2">
+        <v>3.4663865546218489</v>
+      </c>
+      <c r="S2">
+        <v>25.358619012885971</v>
+      </c>
+      <c r="T2">
+        <v>52.714535901926439</v>
+      </c>
+      <c r="U2">
+        <v>25.183374083129586</v>
+      </c>
+      <c r="V2">
+        <v>36.381938452689099</v>
+      </c>
+      <c r="W2">
+        <v>16.909620991253643</v>
+      </c>
+      <c r="X2">
+        <v>25.790921595598348</v>
+      </c>
+      <c r="Y2">
+        <v>35.565356856455494</v>
+      </c>
+      <c r="Z2">
+        <v>6.8690754224481383</v>
+      </c>
+      <c r="AA2">
+        <v>5.0539466212379329</v>
+      </c>
+      <c r="AB2">
+        <v>11.494252873563218</v>
+      </c>
+      <c r="AC2">
+        <v>33.93333333333333</v>
+      </c>
+      <c r="AD2">
+        <v>20.257782101167315</v>
+      </c>
+      <c r="AE2">
+        <v>65.460526315789465</v>
+      </c>
+      <c r="AF2">
+        <v>20.78239608801956</v>
+      </c>
+      <c r="AH2">
+        <v>22.846441947565545</v>
+      </c>
+      <c r="AI2">
+        <v>0.86812732534105008</v>
+      </c>
+      <c r="AJ2">
+        <v>39.148936170212764</v>
+      </c>
+      <c r="AK2">
+        <v>15.131578947368421</v>
+      </c>
+      <c r="AL2">
+        <v>12.701298701298702</v>
+      </c>
+      <c r="AM2">
+        <v>54.093050647820959</v>
+      </c>
+      <c r="AN2">
+        <v>21.055634807417974</v>
+      </c>
+      <c r="AO2">
+        <v>28.972917731221258</v>
+      </c>
+      <c r="AP2">
+        <v>8.2442748091603058</v>
+      </c>
+      <c r="AQ2">
+        <v>8.0474111041796643</v>
+      </c>
+      <c r="AR2">
+        <v>14.372822299651569</v>
+      </c>
+      <c r="AS2">
+        <v>33.558178752107928</v>
+      </c>
+      <c r="AT2">
+        <v>12.231954092419208</v>
+      </c>
+      <c r="AU2">
+        <v>36.73770491803279</v>
+      </c>
+      <c r="AV2">
+        <v>16.251556662515569</v>
+      </c>
+      <c r="AX2">
+        <v>9.9188458070333638</v>
+      </c>
+      <c r="AY2">
+        <v>31.716417910447763</v>
+      </c>
+      <c r="AZ2">
+        <v>17.870129870129869</v>
+      </c>
+      <c r="BA2">
+        <v>27.640918580375782</v>
+      </c>
+      <c r="BB2">
+        <v>11.263020833333332</v>
+      </c>
+      <c r="BC2">
+        <v>29.015544041450774</v>
+      </c>
+      <c r="BD2">
+        <v>54.632587859424916</v>
+      </c>
+      <c r="BE2">
+        <v>52.589936951415503</v>
+      </c>
+      <c r="BF2">
+        <v>19.423368740515933</v>
+      </c>
+      <c r="BG2">
+        <v>13.911326512295819</v>
+      </c>
+      <c r="BH2">
+        <v>29.810008027829809</v>
+      </c>
+      <c r="BI2">
+        <v>33.576642335766422</v>
+      </c>
+      <c r="BJ2">
+        <v>12.842278203723986</v>
+      </c>
+      <c r="BK2">
+        <v>94.444444444444443</v>
+      </c>
+      <c r="BL2">
+        <v>18.387293830177153</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3725,12 +4143,485 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>641</v>
+      </c>
+      <c r="B2">
+        <v>65.460526315789465</v>
+      </c>
+      <c r="E2" s="9">
+        <v>656</v>
+      </c>
+      <c r="F2">
+        <v>16.251556662515569</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>520</v>
+      </c>
+      <c r="B3">
+        <v>6.2124248496993983</v>
+      </c>
+      <c r="E3" s="6">
+        <v>634</v>
+      </c>
+      <c r="F3">
+        <v>11.263020833333332</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>500</v>
+      </c>
+      <c r="B4">
+        <v>52.589936951415503</v>
+      </c>
+      <c r="E4" s="9">
+        <v>620</v>
+      </c>
+      <c r="F4">
+        <v>36.73770491803279</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>426</v>
+      </c>
+      <c r="B5">
+        <v>94.444444444444443</v>
+      </c>
+      <c r="E5" s="6">
+        <v>617</v>
+      </c>
+      <c r="F5">
+        <v>12.231954092419208</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>414</v>
+      </c>
+      <c r="B6">
+        <v>31.716417910447763</v>
+      </c>
+      <c r="E6" s="9">
+        <v>616</v>
+      </c>
+      <c r="F6">
+        <v>33.558178752107928</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>364</v>
+      </c>
+      <c r="B7">
+        <v>54.632587859424916</v>
+      </c>
+      <c r="E7" s="9">
+        <v>608</v>
+      </c>
+      <c r="F7">
+        <v>18.52367688022284</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>321</v>
+      </c>
+      <c r="B8">
+        <v>29.810008027829809</v>
+      </c>
+      <c r="E8" s="6">
+        <v>603</v>
+      </c>
+      <c r="F8">
+        <v>27.640918580375782</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>206</v>
+      </c>
+      <c r="B9">
+        <v>27.860696517412936</v>
+      </c>
+      <c r="E9" s="6">
+        <v>599</v>
+      </c>
+      <c r="F9">
+        <v>18.387293830177153</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>189</v>
+      </c>
+      <c r="B10">
+        <v>14.437760296159185</v>
+      </c>
+      <c r="E10" s="6">
+        <v>587</v>
+      </c>
+      <c r="F10">
+        <v>20.78239608801956</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E11" s="9">
+        <v>572</v>
+      </c>
+      <c r="F11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E12" s="6">
+        <v>533</v>
+      </c>
+      <c r="F12">
+        <v>14.372822299651569</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E13" s="9">
+        <v>529</v>
+      </c>
+      <c r="F13">
+        <v>20.257782101167315</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E14" s="9">
+        <v>513</v>
+      </c>
+      <c r="F14">
+        <v>8.0474111041796643</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E15" s="9">
+        <v>487</v>
+      </c>
+      <c r="F15">
+        <v>8.2442748091603058</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E16" s="9">
+        <v>481</v>
+      </c>
+      <c r="F16">
+        <v>12.558548009367682</v>
+      </c>
+    </row>
+    <row r="17" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E17" s="6">
+        <v>472</v>
+      </c>
+      <c r="F17">
+        <v>17.870129870129869</v>
+      </c>
+    </row>
+    <row r="18" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E18" s="6">
+        <v>470</v>
+      </c>
+      <c r="F18">
+        <v>28.972917731221258</v>
+      </c>
+    </row>
+    <row r="19" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E19" s="6">
+        <v>465</v>
+      </c>
+      <c r="F19">
+        <v>13.043478260869565</v>
+      </c>
+    </row>
+    <row r="20" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E20" s="6">
+        <v>413</v>
+      </c>
+      <c r="F20">
+        <v>33.93333333333333</v>
+      </c>
+    </row>
+    <row r="21" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E21" s="9">
+        <v>408</v>
+      </c>
+      <c r="F21">
+        <v>21.055634807417974</v>
+      </c>
+    </row>
+    <row r="22" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E22" s="9">
+        <v>395</v>
+      </c>
+      <c r="F22">
+        <v>11.494252873563218</v>
+      </c>
+    </row>
+    <row r="23" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E23" s="6">
+        <v>382</v>
+      </c>
+      <c r="F23">
+        <v>54.093050647820959</v>
+      </c>
+    </row>
+    <row r="24" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E24" s="9">
+        <v>353</v>
+      </c>
+      <c r="F24">
+        <v>5.0539466212379329</v>
+      </c>
+    </row>
+    <row r="25" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E25" s="11">
+        <v>347</v>
+      </c>
+      <c r="F25">
+        <v>12.842278203723986</v>
+      </c>
+    </row>
+    <row r="26" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E26" s="11">
+        <v>346</v>
+      </c>
+      <c r="F26">
+        <v>33.576642335766422</v>
+      </c>
+    </row>
+    <row r="27" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E27" s="6">
+        <v>342</v>
+      </c>
+      <c r="F27">
+        <v>35.61463543037641</v>
+      </c>
+    </row>
+    <row r="28" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E28" s="9">
+        <v>341</v>
+      </c>
+      <c r="F28">
+        <v>12.701298701298702</v>
+      </c>
+    </row>
+    <row r="29" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E29" s="9">
+        <v>301</v>
+      </c>
+      <c r="F29">
+        <v>6.8690754224481383</v>
+      </c>
+    </row>
+    <row r="30" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E30" s="9">
+        <v>295</v>
+      </c>
+      <c r="F30">
+        <v>35.565356856455494</v>
+      </c>
+    </row>
+    <row r="31" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E31" s="9">
+        <v>282</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E32" s="6">
+        <v>271</v>
+      </c>
+      <c r="F32">
+        <v>7.9720279720279716</v>
+      </c>
+    </row>
+    <row r="33" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E33" s="9">
+        <v>249</v>
+      </c>
+      <c r="F33">
+        <v>25.790921595598348</v>
+      </c>
+    </row>
+    <row r="34" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E34" s="6">
+        <v>244</v>
+      </c>
+      <c r="F34">
+        <v>16.909620991253643</v>
+      </c>
+    </row>
+    <row r="35" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E35" s="6">
+        <v>241</v>
+      </c>
+      <c r="F35">
+        <v>13.911326512295819</v>
+      </c>
+    </row>
+    <row r="36" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E36" s="9">
+        <v>240</v>
+      </c>
+      <c r="F36">
+        <v>47.955145118733512</v>
+      </c>
+    </row>
+    <row r="37" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E37" s="9">
+        <v>228</v>
+      </c>
+      <c r="F37">
+        <v>5.1921079958463139</v>
+      </c>
+    </row>
+    <row r="38" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E38" s="6">
+        <v>190</v>
+      </c>
+      <c r="F38">
+        <v>36.381938452689099</v>
+      </c>
+    </row>
+    <row r="39" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E39" s="6">
+        <v>168</v>
+      </c>
+      <c r="F39">
+        <v>15.131578947368421</v>
+      </c>
+    </row>
+    <row r="40" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E40" s="6">
+        <v>148</v>
+      </c>
+      <c r="F40">
+        <v>29.015544041450774</v>
+      </c>
+    </row>
+    <row r="41" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E41" s="6">
+        <v>126</v>
+      </c>
+      <c r="F41">
+        <v>19.423368740515933</v>
+      </c>
+    </row>
+    <row r="42" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E42" s="9">
+        <v>122</v>
+      </c>
+      <c r="F42">
+        <v>8.615384615384615</v>
+      </c>
+    </row>
+    <row r="43" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E43" s="6">
+        <v>98</v>
+      </c>
+      <c r="F43">
+        <v>39.148936170212764</v>
+      </c>
+    </row>
+    <row r="44" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E44" s="6">
+        <v>97</v>
+      </c>
+      <c r="F44">
+        <v>25.183374083129586</v>
+      </c>
+    </row>
+    <row r="45" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E45" s="9">
+        <v>92</v>
+      </c>
+      <c r="F45">
+        <v>10.632610632610632</v>
+      </c>
+    </row>
+    <row r="46" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E46" s="9">
+        <v>89</v>
+      </c>
+      <c r="F46">
+        <v>0.86812732534105008</v>
+      </c>
+    </row>
+    <row r="47" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E47" s="6">
+        <v>70</v>
+      </c>
+      <c r="F47">
+        <v>52.714535901926439</v>
+      </c>
+    </row>
+    <row r="48" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E48" s="9">
+        <v>65</v>
+      </c>
+      <c r="F48">
+        <v>13.116057233704293</v>
+      </c>
+    </row>
+    <row r="49" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E49" s="6">
+        <v>52</v>
+      </c>
+      <c r="F49">
+        <v>22.846441947565545</v>
+      </c>
+    </row>
+    <row r="50" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E50" s="6">
+        <v>36</v>
+      </c>
+      <c r="F50">
+        <v>25.358619012885971</v>
+      </c>
+    </row>
+    <row r="51" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E51" s="6">
+        <v>28</v>
+      </c>
+      <c r="F51">
+        <v>9.9188458070333638</v>
+      </c>
+    </row>
+    <row r="52" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E52" s="9">
+        <v>26</v>
+      </c>
+      <c r="F52">
+        <v>3.4663865546218489</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>